<commit_message>
refactor: Remove orçamento, finanças e indicadores de saúde do projeto
</commit_message>
<xml_diff>
--- a/Planilha_Tradicional_GGOV.xlsx
+++ b/Planilha_Tradicional_GGOV.xlsx
@@ -559,11 +559,6 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Orçamento</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
           <t>Descrição</t>
         </is>
       </c>
@@ -591,11 +586,6 @@
         <v>46053</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>R$ 15.000</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Realizar o mapeamento completo dos processos administrativos e operacionais do GGOV</t>
         </is>

</xml_diff>